<commit_message>
Added Data mol vs biomass vs total accumlated water
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25930"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C5ADFBD-7FEA-4D1C-8B18-9B0EBCA1CA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B49B12C-F5CA-4E67-8C41-0F3502ED9122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="water_times" sheetId="3" r:id="rId1"/>
     <sheet name="water_flow" sheetId="1" r:id="rId2"/>
     <sheet name="radiation" sheetId="2" r:id="rId3"/>
     <sheet name="biomass" sheetId="4" r:id="rId4"/>
+    <sheet name="accumulated_water_light" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="22">
   <si>
     <t>on</t>
   </si>
@@ -112,12 +113,27 @@
       <t>-1</t>
     </r>
   </si>
+  <si>
+    <t>accumlated_water</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>mol</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +151,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="ArialMT"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -158,9 +180,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4A225B4-469F-4702-806B-983FF8A18401}">
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76:C84"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1720,4 +1743,1707 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BDC2C51-5A20-4493-A0E6-DCB2FC49AD1F}">
+  <dimension ref="A1:C153"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140:C153"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2">
+        <v>0.244225299699635</v>
+      </c>
+      <c r="B3" s="2">
+        <v>66.226309773796004</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2">
+        <v>0.488477180298237</v>
+      </c>
+      <c r="B4" s="2">
+        <v>132.37287685069501</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2">
+        <v>0.74181972834321197</v>
+      </c>
+      <c r="B5" s="2">
+        <v>198.532734377076</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2">
+        <v>1.04061561362005</v>
+      </c>
+      <c r="B6" s="2">
+        <v>264.75904415087302</v>
+      </c>
+      <c r="C6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2">
+        <v>1.2845485234310601</v>
+      </c>
+      <c r="B7" s="2">
+        <v>348.44900454533303</v>
+      </c>
+      <c r="C7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="2">
+        <v>1.51978947928019</v>
+      </c>
+      <c r="B8" s="2">
+        <v>410.19643284335899</v>
+      </c>
+      <c r="C8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="2">
+        <v>1.74570053959225</v>
+      </c>
+      <c r="B9" s="2">
+        <v>485.08811568007201</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="2">
+        <v>1.99019164828154</v>
+      </c>
+      <c r="B10" s="2">
+        <v>538.07713776879905</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="2">
+        <v>2.2526248637728901</v>
+      </c>
+      <c r="B11" s="2">
+        <v>604.25028574466398</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="2">
+        <v>2.4692060285478901</v>
+      </c>
+      <c r="B12" s="2">
+        <v>692.28622312006598</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="2">
+        <v>2.68626564950427</v>
+      </c>
+      <c r="B13" s="2">
+        <v>754.00707051912502</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="2">
+        <v>3.0034820977645502</v>
+      </c>
+      <c r="B14" s="2">
+        <v>807.10241620371596</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="2">
+        <v>3.2020414130405901</v>
+      </c>
+      <c r="B15" s="2">
+        <v>886.34007602137103</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="2">
+        <v>3.4825762207277799</v>
+      </c>
+      <c r="B16" s="2">
+        <v>956.92565322559199</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2">
+        <v>3.6996358416841701</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1018.64650062465</v>
+      </c>
+      <c r="C17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="2">
+        <v>3.9894208022115301</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1080.47367161957</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="2">
+        <v>4.2335929401132404</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1151.0060870258601</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2">
+        <v>4.4775258499242501</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1234.6960474203199</v>
+      </c>
+      <c r="C20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="2">
+        <v>0.26041306716993101</v>
+      </c>
+      <c r="B21" s="2">
+        <v>175.899098907525</v>
+      </c>
+      <c r="C21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="2">
+        <v>0.48624438478509302</v>
+      </c>
+      <c r="B22" s="2">
+        <v>255.17663007362799</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="2">
+        <v>0.73910847664867996</v>
+      </c>
+      <c r="B23" s="2">
+        <v>347.65157757635302</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="2">
+        <v>0.91924722894128297</v>
+      </c>
+      <c r="B24" s="2">
+        <v>440.02020148321401</v>
+      </c>
+      <c r="C24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="2">
+        <v>4.7039153664176903</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1283.27264028069</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2">
+        <v>4.9845299168017903</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1349.47236915552</v>
+      </c>
+      <c r="C26">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="2">
+        <v>5.1828500039871299</v>
+      </c>
+      <c r="B27" s="2">
+        <v>1441.86757396135</v>
+      </c>
+      <c r="C27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="2">
+        <v>5.5001461949443096</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1490.57707131655</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="2">
+        <v>5.74447781823981</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1552.3377900640601</v>
+      </c>
+      <c r="C29">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2">
+        <v>5.97030913585498</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1631.6153212301599</v>
+      </c>
+      <c r="C30">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="2">
+        <v>6.2144812737566797</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1702.14773663645</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="2">
+        <v>6.51335690173042</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1763.98819808086</v>
+      </c>
+      <c r="C32">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2">
+        <v>6.7212461125435299</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1830.0816033598301</v>
+      </c>
+      <c r="C33">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2">
+        <v>7.0016214348369301</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1909.4388772228299</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2">
+        <v>7.2458733154355297</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1975.5854442997299</v>
+      </c>
+      <c r="C35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2">
+        <v>7.4359799048403801</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2019.72302703277</v>
+      </c>
+      <c r="C36">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2">
+        <v>7.7165147125275801</v>
+      </c>
+      <c r="B37" s="2">
+        <v>2090.3086042370001</v>
+      </c>
+      <c r="C37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2">
+        <v>8.0060604449642501</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2165.2933202200902</v>
+      </c>
+      <c r="C38">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="2">
+        <v>8.2413811435102708</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2222.6549001887302</v>
+      </c>
+      <c r="C39">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="2">
+        <v>8.5128252837511003</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2293.2271869434599</v>
+      </c>
+      <c r="C40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2">
+        <v>8.7385768586693597</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2376.8905664389599</v>
+      </c>
+      <c r="C41">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2">
+        <v>0.28138539645410798</v>
+      </c>
+      <c r="B42" s="2">
+        <v>22.420988277823199</v>
+      </c>
+      <c r="C42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2">
+        <v>0.50721671406926905</v>
+      </c>
+      <c r="B43" s="2">
+        <v>101.698519443927</v>
+      </c>
+      <c r="C43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2">
+        <v>0.76901198798543302</v>
+      </c>
+      <c r="B44" s="2">
+        <v>202.95845405491499</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2">
+        <v>0.99500279099439104</v>
+      </c>
+      <c r="B45" s="2">
+        <v>273.46428856223901</v>
+      </c>
+      <c r="C45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2">
+        <v>1.24786688285798</v>
+      </c>
+      <c r="B46" s="2">
+        <v>365.93923606496401</v>
+      </c>
+      <c r="C46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2">
+        <v>1.5101406129555299</v>
+      </c>
+      <c r="B47" s="2">
+        <v>440.884080699609</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2">
+        <v>1.73645038675208</v>
+      </c>
+      <c r="B48" s="2">
+        <v>493.84652188937002</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2">
+        <v>1.98931447861567</v>
+      </c>
+      <c r="B49" s="2">
+        <v>586.32146939209497</v>
+      </c>
+      <c r="C49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2">
+        <v>2.2339650726987599</v>
+      </c>
+      <c r="B50" s="2">
+        <v>630.53879482204104</v>
+      </c>
+      <c r="C50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="2">
+        <v>2.5231918343478399</v>
+      </c>
+      <c r="B51" s="2">
+        <v>723.066904122697</v>
+      </c>
+      <c r="C51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="2">
+        <v>2.7310810451609502</v>
+      </c>
+      <c r="B52" s="2">
+        <v>789.16030940166399</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="2">
+        <v>2.98418436511523</v>
+      </c>
+      <c r="B53" s="2">
+        <v>868.477711916217</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="2">
+        <v>3.2647989154993202</v>
+      </c>
+      <c r="B54" s="2">
+        <v>934.67744079104796</v>
+      </c>
+      <c r="C54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="2">
+        <v>3.4995614151670602</v>
+      </c>
+      <c r="B55" s="2">
+        <v>1022.73995906542</v>
+      </c>
+      <c r="C55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="2">
+        <v>3.7256319608729198</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1088.85994524335</v>
+      </c>
+      <c r="C56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="2">
+        <v>3.9879854336673701</v>
+      </c>
+      <c r="B57" s="2">
+        <v>1159.4189415486001</v>
+      </c>
+      <c r="C57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2">
+        <v>4.2413279817123399</v>
+      </c>
+      <c r="B58" s="2">
+        <v>1225.57879907499</v>
+      </c>
+      <c r="C58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="2">
+        <v>4.4943515589697203</v>
+      </c>
+      <c r="B59" s="2">
+        <v>1309.2820499189299</v>
+      </c>
+      <c r="C59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="2">
+        <v>4.7476143643178004</v>
+      </c>
+      <c r="B60" s="2">
+        <v>1379.8277557747001</v>
+      </c>
+      <c r="C60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="2">
+        <v>4.9734456819329598</v>
+      </c>
+      <c r="B61" s="2">
+        <v>1459.1052869407999</v>
+      </c>
+      <c r="C61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="2">
+        <v>5.2173785917439801</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1542.79524733527</v>
+      </c>
+      <c r="C62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="2">
+        <v>5.4798118072353201</v>
+      </c>
+      <c r="B63" s="2">
+        <v>1608.9683953111301</v>
+      </c>
+      <c r="C63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="2">
+        <v>5.7060418383349703</v>
+      </c>
+      <c r="B64" s="2">
+        <v>1666.3166848302801</v>
+      </c>
+      <c r="C64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="2">
+        <v>5.9861779325376796</v>
+      </c>
+      <c r="B65" s="2">
+        <v>1758.8315036814499</v>
+      </c>
+      <c r="C65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2">
+        <v>6.2575423300816002</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1833.7896387655801</v>
+      </c>
+      <c r="C66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="2">
+        <v>6.4651923128040201</v>
+      </c>
+      <c r="B67" s="2">
+        <v>1913.0405890327199</v>
+      </c>
+      <c r="C67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="2">
+        <v>6.7186146035458902</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1974.8145982297101</v>
+      </c>
+      <c r="C68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="2">
+        <v>6.9805693628558503</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2067.3028361819202</v>
+      </c>
+      <c r="C69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="2">
+        <v>7.2156508333111802</v>
+      </c>
+      <c r="B70" s="2">
+        <v>2137.8219611387299</v>
+      </c>
+      <c r="C70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="2">
+        <v>7.45081204646341</v>
+      </c>
+      <c r="B71" s="2">
+        <v>2203.9552377661398</v>
+      </c>
+      <c r="C71">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="2">
+        <v>7.7311076260599201</v>
+      </c>
+      <c r="B72" s="2">
+        <v>2287.6983599585301</v>
+      </c>
+      <c r="C72">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="2">
+        <v>0.25108317163286398</v>
+      </c>
+      <c r="B73" s="2">
+        <v>189.04335344621299</v>
+      </c>
+      <c r="C73">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2">
+        <v>0.51303793094282402</v>
+      </c>
+      <c r="B74" s="2">
+        <v>281.53159139842001</v>
+      </c>
+      <c r="C74">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="2">
+        <v>0.73855027777039395</v>
+      </c>
+      <c r="B75" s="2">
+        <v>378.35251588208598</v>
+      </c>
+      <c r="C75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="2">
+        <v>1.0188458573668999</v>
+      </c>
+      <c r="B76" s="2">
+        <v>462.09563807447898</v>
+      </c>
+      <c r="C76">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="2">
+        <v>1.2628585098748</v>
+      </c>
+      <c r="B77" s="2">
+        <v>541.39975013954904</v>
+      </c>
+      <c r="C77">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="2">
+        <v>1.5158820871321901</v>
+      </c>
+      <c r="B78" s="2">
+        <v>625.10300098349296</v>
+      </c>
+      <c r="C78">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="2">
+        <v>1.75048510140613</v>
+      </c>
+      <c r="B79" s="2">
+        <v>721.937215916642</v>
+      </c>
+      <c r="C79">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="2">
+        <v>1.9942585258233401</v>
+      </c>
+      <c r="B80" s="2">
+        <v>814.398872969884</v>
+      </c>
+      <c r="C80">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="2">
+        <v>2.2469631322931298</v>
+      </c>
+      <c r="B81" s="2">
+        <v>915.64551713138906</v>
+      </c>
+      <c r="C81">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2">
+        <v>2.5179288163525699</v>
+      </c>
+      <c r="B82" s="2">
+        <v>1012.53289386247</v>
+      </c>
+      <c r="C82">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="2">
+        <v>2.7350681800058498</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1069.86789293214</v>
+      </c>
+      <c r="C83">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="2">
+        <v>2.9605007841365198</v>
+      </c>
+      <c r="B84" s="2">
+        <v>1171.0746657452</v>
+      </c>
+      <c r="C84">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="2">
+        <v>3.2498870311793899</v>
+      </c>
+      <c r="B85" s="2">
+        <v>1254.83107838707</v>
+      </c>
+      <c r="C85">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="2">
+        <v>3.4656707689854098</v>
+      </c>
+      <c r="B86" s="2">
+        <v>1386.7254990563799</v>
+      </c>
+      <c r="C86">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="2">
+        <v>3.7553759868158698</v>
+      </c>
+      <c r="B87" s="2">
+        <v>1452.9385183806901</v>
+      </c>
+      <c r="C87">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="2">
+        <v>4.0078413651949703</v>
+      </c>
+      <c r="B88" s="2">
+        <v>1567.34270753037</v>
+      </c>
+      <c r="C88">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="2">
+        <v>4.2339119109008303</v>
+      </c>
+      <c r="B89" s="2">
+        <v>1633.4626937083001</v>
+      </c>
+      <c r="C89">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2">
+        <v>4.4685946678716704</v>
+      </c>
+      <c r="B90" s="2">
+        <v>1725.91106031206</v>
+      </c>
+      <c r="C90">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="2">
+        <v>4.7124478349857801</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1813.9868690359101</v>
+      </c>
+      <c r="C91">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="2">
+        <v>4.9559820313123</v>
+      </c>
+      <c r="B92" s="2">
+        <v>1919.6060710773199</v>
+      </c>
+      <c r="C92">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="2">
+        <v>5.2271072007655297</v>
+      </c>
+      <c r="B93" s="2">
+        <v>2007.7217511496201</v>
+      </c>
+      <c r="C93">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="2">
+        <v>5.4798915499322201</v>
+      </c>
+      <c r="B94" s="2">
+        <v>2104.5825469817401</v>
+      </c>
+      <c r="C94">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="2">
+        <v>5.6965524574041098</v>
+      </c>
+      <c r="B95" s="2">
+        <v>2188.2326360277498</v>
+      </c>
+      <c r="C95">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="2">
+        <v>5.9585869594109697</v>
+      </c>
+      <c r="B96" s="2">
+        <v>2276.3350256505701</v>
+      </c>
+      <c r="C96">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="2">
+        <v>6.22030249063023</v>
+      </c>
+      <c r="B97" s="2">
+        <v>2381.9808085909499</v>
+      </c>
+      <c r="C97">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2">
+        <v>6.4461338082454001</v>
+      </c>
+      <c r="B98" s="2">
+        <v>2461.2583397570502</v>
+      </c>
+      <c r="C98">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="2">
+        <v>0.259854868291645</v>
+      </c>
+      <c r="B99" s="2">
+        <v>206.60003721325799</v>
+      </c>
+      <c r="C99">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="2">
+        <v>0.49445788256558798</v>
+      </c>
+      <c r="B100" s="2">
+        <v>303.434252146407</v>
+      </c>
+      <c r="C100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="2">
+        <v>0.738151564285904</v>
+      </c>
+      <c r="B101" s="2">
+        <v>400.281757529039</v>
+      </c>
+      <c r="C101">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="2">
+        <v>1.03583105180617</v>
+      </c>
+      <c r="B102" s="2">
+        <v>527.90994391430297</v>
+      </c>
+      <c r="C102">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="2">
+        <v>1.2613433986337399</v>
+      </c>
+      <c r="B103" s="2">
+        <v>624.73086839796895</v>
+      </c>
+      <c r="C103">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="2">
+        <v>1.4872544589458001</v>
+      </c>
+      <c r="B104" s="2">
+        <v>699.62255123468196</v>
+      </c>
+      <c r="C104">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="2">
+        <v>1.703676138327</v>
+      </c>
+      <c r="B105" s="2">
+        <v>796.43018526886499</v>
+      </c>
+      <c r="C105">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="2">
+        <v>1.9744025942957399</v>
+      </c>
+      <c r="B106" s="2">
+        <v>906.475106988118</v>
+      </c>
+      <c r="C106">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="2">
+        <v>2.2180165333191599</v>
+      </c>
+      <c r="B107" s="2">
+        <v>1007.70846070014</v>
+      </c>
+      <c r="C107">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="2">
+        <v>2.4890619600754902</v>
+      </c>
+      <c r="B108" s="2">
+        <v>1100.2099891018299</v>
+      </c>
+      <c r="C108">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="2">
+        <v>2.7235054889556398</v>
+      </c>
+      <c r="B109" s="2">
+        <v>1205.8159006937601</v>
+      </c>
+      <c r="C109">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="2">
+        <v>2.9943116876212801</v>
+      </c>
+      <c r="B110" s="2">
+        <v>1311.4749740836201</v>
+      </c>
+      <c r="C110">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="2">
+        <v>3.2561069615374398</v>
+      </c>
+      <c r="B111" s="2">
+        <v>1412.7349086946101</v>
+      </c>
+      <c r="C111">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="2">
+        <v>3.4726881263124301</v>
+      </c>
+      <c r="B112" s="2">
+        <v>1500.7708460700101</v>
+      </c>
+      <c r="C112">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="2">
+        <v>3.7250737619946301</v>
+      </c>
+      <c r="B113" s="2">
+        <v>1619.56088354908</v>
+      </c>
+      <c r="C113">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="2">
+        <v>4.0049706281066397</v>
+      </c>
+      <c r="B114" s="2">
+        <v>1725.2332473884301</v>
+      </c>
+      <c r="C114">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="2">
+        <v>4.2217112782754302</v>
+      </c>
+      <c r="B115" s="2">
+        <v>1804.49748810505</v>
+      </c>
+      <c r="C115">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="2">
+        <v>4.4559953217617796</v>
+      </c>
+      <c r="B116" s="2">
+        <v>1918.87509635576</v>
+      </c>
+      <c r="C116">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="2">
+        <v>4.7268015204274203</v>
+      </c>
+      <c r="B117" s="2">
+        <v>2024.5341697456199</v>
+      </c>
+      <c r="C117">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="2">
+        <v>4.9522341245580899</v>
+      </c>
+      <c r="B118" s="2">
+        <v>2125.7409425586802</v>
+      </c>
+      <c r="C118">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="2">
+        <v>5.2503920682597496</v>
+      </c>
+      <c r="B119" s="2">
+        <v>2227.0540389675998</v>
+      </c>
+      <c r="C119">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="2">
+        <v>5.5127455410542003</v>
+      </c>
+      <c r="B120" s="2">
+        <v>2297.6130352728501</v>
+      </c>
+      <c r="C120">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="2">
+        <v>0.28688764254006999</v>
+      </c>
+      <c r="B121" s="2">
+        <v>219.79745354987801</v>
+      </c>
+      <c r="C121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="2">
+        <v>0.51263921745833396</v>
+      </c>
+      <c r="B122" s="2">
+        <v>303.46083304537302</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="2">
+        <v>0.77491294755588602</v>
+      </c>
+      <c r="B123" s="2">
+        <v>378.40567768001802</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="2">
+        <v>1.0188458573668999</v>
+      </c>
+      <c r="B124" s="2">
+        <v>462.09563807447898</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="2">
+        <v>1.25352861433774</v>
+      </c>
+      <c r="B125" s="2">
+        <v>554.54400467823803</v>
+      </c>
+      <c r="C125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="2">
+        <v>1.4697110656282399</v>
+      </c>
+      <c r="B126" s="2">
+        <v>664.50918370059298</v>
+      </c>
+      <c r="C126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="2">
+        <v>1.7405970069907799</v>
+      </c>
+      <c r="B127" s="2">
+        <v>765.78240876106395</v>
+      </c>
+      <c r="C127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="2">
+        <v>2.0027112516945298</v>
+      </c>
+      <c r="B128" s="2">
+        <v>849.49895005449002</v>
+      </c>
+      <c r="C128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="2">
+        <v>2.2192924164695298</v>
+      </c>
+      <c r="B129" s="2">
+        <v>937.53488742989305</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="2">
+        <v>2.5173706174742798</v>
+      </c>
+      <c r="B130" s="2">
+        <v>1043.2338321682</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="2">
+        <v>2.7432019350894401</v>
+      </c>
+      <c r="B131" s="2">
+        <v>1122.5113633343101</v>
+      </c>
+      <c r="C131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="2">
+        <v>3.0140081337550799</v>
+      </c>
+      <c r="B132" s="2">
+        <v>1228.17043672417</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="2">
+        <v>3.2577815581723</v>
+      </c>
+      <c r="B133" s="2">
+        <v>1320.6320937774101</v>
+      </c>
+      <c r="C133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="2">
+        <v>3.46527205550092</v>
+      </c>
+      <c r="B134" s="2">
+        <v>1408.6547407033299</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="2">
+        <v>3.7091252226150302</v>
+      </c>
+      <c r="B135" s="2">
+        <v>1496.73054942718</v>
+      </c>
+      <c r="C135">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="2">
+        <v>3.9710799819249898</v>
+      </c>
+      <c r="B136" s="2">
+        <v>1589.2187873793901</v>
+      </c>
+      <c r="C136">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="2">
+        <v>4.2422051513782204</v>
+      </c>
+      <c r="B137" s="2">
+        <v>1677.33446745169</v>
+      </c>
+      <c r="C137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="2">
+        <v>4.4493766779192496</v>
+      </c>
+      <c r="B138" s="2">
+        <v>1782.9005076951701</v>
+      </c>
+      <c r="C138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="2">
+        <v>4.7570240025517698</v>
+      </c>
+      <c r="B139" s="2">
+        <v>1862.29765290662</v>
+      </c>
+      <c r="C139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="2">
+        <v>0.286249700964886</v>
+      </c>
+      <c r="B140" s="2">
+        <v>254.884240185002</v>
+      </c>
+      <c r="C140">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="2">
+        <v>0.47516014991626898</v>
+      </c>
+      <c r="B141" s="2">
+        <v>364.80954785890799</v>
+      </c>
+      <c r="C141">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="2">
+        <v>0.74540814970362301</v>
+      </c>
+      <c r="B142" s="2">
+        <v>501.169559554503</v>
+      </c>
+      <c r="C142">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="2">
+        <v>1.0163738337630599</v>
+      </c>
+      <c r="B143" s="2">
+        <v>598.05693628558504</v>
+      </c>
+      <c r="C143">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="2">
+        <v>1.2325562850535601</v>
+      </c>
+      <c r="B144" s="2">
+        <v>708.02211530793898</v>
+      </c>
+      <c r="C144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="2">
+        <v>1.5028840275378099</v>
+      </c>
+      <c r="B145" s="2">
+        <v>839.99627867414495</v>
+      </c>
+      <c r="C145">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="2">
+        <v>1.76475904415087</v>
+      </c>
+      <c r="B146" s="2">
+        <v>936.87036495574296</v>
+      </c>
+      <c r="C146">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="2">
+        <v>1.9537492357991499</v>
+      </c>
+      <c r="B147" s="2">
+        <v>1042.40982430026</v>
+      </c>
+      <c r="C147">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="2">
+        <v>2.2155445097153201</v>
+      </c>
+      <c r="B148" s="2">
+        <v>1143.66975891125</v>
+      </c>
+      <c r="C148">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="2">
+        <v>2.49496291964594</v>
+      </c>
+      <c r="B149" s="2">
+        <v>1275.6572127269301</v>
+      </c>
+      <c r="C149">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="2">
+        <v>2.6840328539911198</v>
+      </c>
+      <c r="B150" s="2">
+        <v>1376.8108237420599</v>
+      </c>
+      <c r="C150">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="2">
+        <v>2.9727014167619101</v>
+      </c>
+      <c r="B151" s="2">
+        <v>1500.0398713484501</v>
+      </c>
+      <c r="C151">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="2">
+        <v>3.2524387974801301</v>
+      </c>
+      <c r="B152" s="2">
+        <v>1614.4839318465799</v>
+      </c>
+      <c r="C152">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="2">
+        <v>3.4685415060737399</v>
+      </c>
+      <c r="B153" s="2">
+        <v>1728.8349591983199</v>
+      </c>
+      <c r="C153">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>